<commit_message>
BOT-538 better quessing mode
</commit_message>
<xml_diff>
--- a/test/compiler/convos/convos_2convos_simplified_to_force.xlsx
+++ b/test/compiler/convos/convos_2convos_simplified_to_force.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>User</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>test 1</t>
-  </si>
-  <si>
-    <t>test 3</t>
   </si>
   <si>
     <t>test 4</t>
@@ -391,7 +388,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -413,18 +410,15 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -432,10 +426,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>